<commit_message>
add test for parameter type
</commit_message>
<xml_diff>
--- a/test/fixtures/files/product_keyword_parameter_test.xlsx
+++ b/test/fixtures/files/product_keyword_parameter_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,27 +15,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>tuotenumero</t>
   </si>
   <si>
-    <t>Tuotteen koko</t>
-  </si>
-  <si>
-    <t>Tuotteen materiaali</t>
-  </si>
-  <si>
-    <t>toiminto</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>kissa</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>Tuotteen väri</t>
+  </si>
+  <si>
+    <t>Malliston nimi</t>
+  </si>
+  <si>
+    <t>poista</t>
+  </si>
+  <si>
+    <t>hammer123</t>
+  </si>
+  <si>
+    <t>musta</t>
+  </si>
+  <si>
+    <t>deluxe</t>
+  </si>
+  <si>
+    <t>helmet123</t>
+  </si>
+  <si>
+    <t>sininen</t>
+  </si>
+  <si>
+    <t>sale</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>ski1</t>
+  </si>
+  <si>
+    <t>valkoinen</t>
+  </si>
+  <si>
+    <t>winter</t>
   </si>
 </sst>
 </file>
@@ -132,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -168,22 +189,38 @@
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>10</v>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>